<commit_message>
[Resource Manager] Add Performance Field for Host
</commit_message>
<xml_diff>
--- a/etc/hostInfo_template.xlsx
+++ b/etc/hostInfo_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\tiem\micro-api\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\tiem\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD847CA-D596-4732-8000-93F2548652A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B163970-FB83-4B8F-8CA8-7E1BBC3CC363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3800" yWindow="3800" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4760" yWindow="5080" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="主机信息" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>主机名称</t>
   </si>
@@ -82,12 +82,6 @@
     <t>10GE</t>
   </si>
   <si>
-    <t>Compute/Storage</t>
-  </si>
-  <si>
-    <t>[{"name": "vda","capacity": 256,"status": 1, "path": "/"}, {"name": "vdd", "capacity": 512,"status": 0, "path": "/mnt/vdd"}, {"name": "vde","capacity": 1024,"status": 0,"path": "/mnt/vde"}]</t>
-  </si>
-  <si>
     <t>主机2</t>
   </si>
   <si>
@@ -106,9 +100,6 @@
     <t>5.2.0</t>
   </si>
   <si>
-    <t>[{"name": "nvme0p1","capacity": 256,"status": 1, "path": "/"}, {"name": "nvme0p2", "capacity": 1024,"status": 0, "path": "/mnt/path1"}, {"name": "nvme0p3","capacity": 4096,"status": 0,"path": "/mnt/path2"}]</t>
-  </si>
-  <si>
     <t>用户名</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -122,6 +113,62 @@
   </si>
   <si>
     <t>admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Compute</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Storage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>性能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>High</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Low</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主机3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>192.168.56.13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Zone3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rack3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{"name": "vda","capacity": 256,"status": 1, "path": "/", "type": "sata"}, {"name": "vdd", "capacity": 512,"status": 0, "path": "/mnt/vdd", "type":"ssd"}, {"name": "vde","capacity": 1024,"status": 0,"path": "/mnt/vde", "type":"nvme_ssd"}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{"name": "nvme0p1","capacity": 256,"status": 1, "path": "/","type":"nvme_ssd"}, {"name": "nvme0p2", "capacity": 1024,"status": 0, "path": "/mnt/path1", "type": "nvme_ssd"}, {"name": "nvme0p3","capacity": 4096,"status": 0,"path": "/mnt/path2", "type": "nvme_ssd"}]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[{"name": "sda","capacity": 256,"status": 1, "path": "/"}, {"name": "sdb", "capacity": 1024,"status": 0, "path": "/mnt/path1"}, {"name": "sdc","capacity": 4096,"status": 0,"path": "/mnt/path2"}]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -179,11 +226,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -460,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,24 +522,24 @@
     <col min="7" max="7" width="12.33203125" customWidth="1"/>
     <col min="8" max="8" width="10.4140625" customWidth="1"/>
     <col min="9" max="9" width="11.58203125" customWidth="1"/>
-    <col min="10" max="10" width="10.08203125" customWidth="1"/>
-    <col min="11" max="11" width="10.4140625" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="50.9140625" customWidth="1"/>
+    <col min="10" max="10" width="7.58203125" customWidth="1"/>
+    <col min="11" max="11" width="7.25" customWidth="1"/>
+    <col min="13" max="14" width="11.58203125" customWidth="1"/>
+    <col min="15" max="15" width="50.9140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>30</v>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -521,22 +568,25 @@
       <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>32</v>
+      <c r="C2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -562,40 +612,43 @@
       <c r="L2" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
+      <c r="C3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>25</v>
-      </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
       </c>
       <c r="J3">
         <v>16</v>
@@ -606,11 +659,61 @@
       <c r="L3" t="s">
         <v>19</v>
       </c>
-      <c r="M3" t="s">
-        <v>20</v>
+      <c r="M3" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <v>64</v>
+      </c>
+      <c r="L4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Resource Manager] Fix header of template file
</commit_message>
<xml_diff>
--- a/etc/hostInfo_template.xlsx
+++ b/etc/hostInfo_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\tiem\etc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6631AAD6-ABB8-413C-B27B-FB8975FDB870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDDCB81-E9A7-40D3-B38A-BE970AAFA60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4760" yWindow="5080" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="4110" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Host Information" sheetId="1" r:id="rId1"/>
@@ -351,7 +351,7 @@
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>[status: 0 - available, 1 - inused]</t>
+      <t>[status(optional): 0 - available, 1 - reserved]</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -741,7 +741,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,6 +978,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Resource Manager] Add Filted by host traits logic
</commit_message>
<xml_diff>
--- a/etc/hostInfo_template.xlsx
+++ b/etc/hostInfo_template.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\tiem\etc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EF990A-A9C1-400C-958D-59AFB26DEEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="17020"/>
   </bookViews>
   <sheets>
     <sheet name="Host Information" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
   <si>
     <t>Host Name</t>
   </si>
@@ -87,6 +81,54 @@
   </si>
   <si>
     <t>Nic</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">Cluster Purpose
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[Database/
+DataMigration]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Component Purpose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[Compute/Storage/
+Dispatch]</t>
+    </r>
   </si>
   <si>
     <r>
@@ -177,6 +219,9 @@
     <t>10GE</t>
   </si>
   <si>
+    <t>Database</t>
+  </si>
+  <si>
     <t>Compute</t>
   </si>
   <si>
@@ -225,76 +270,26 @@
     <t>Rack3</t>
   </si>
   <si>
-    <t>General</t>
+    <t>Dispatch</t>
   </si>
   <si>
     <t>sata</t>
   </si>
   <si>
     <t>[{"name": "sda","capacity": 256,"status": 1, "path": "/"}, {"name": "sdb", "capacity": 1024,"status": 0, "path": "/mnt/path1"}, {"name": "sdc","capacity": 4096,"status": 0,"path": "/mnt/path2"}]</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>Component Purpose</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>[Compute/Storage/
-Dispatch/General]</t>
-    </r>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Cluster Purpose
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>[Database/
-DataMigration]</t>
-    </r>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Database</t>
-    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="32">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -319,18 +314,196 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -351,55 +524,202 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -407,9 +727,251 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -423,104 +985,80 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -534,7 +1072,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CEEACA"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -778,38 +1316,38 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="1" width="13.9140625" customWidth="1"/>
+    <col min="1" max="1" width="13.9107142857143" customWidth="1"/>
     <col min="2" max="2" width="15.75" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6607142857143" customWidth="1"/>
     <col min="4" max="4" width="14.75" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.3303571428571" customWidth="1"/>
     <col min="6" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.08203125" customWidth="1"/>
-    <col min="9" max="9" width="10.4140625" customWidth="1"/>
+    <col min="8" max="8" width="10.0803571428571" customWidth="1"/>
+    <col min="9" max="9" width="10.4107142857143" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.66071428571429" customWidth="1"/>
     <col min="12" max="12" width="7.25" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" customWidth="1"/>
-    <col min="16" max="16" width="11.58203125" customWidth="1"/>
-    <col min="17" max="17" width="50.9140625" customWidth="1"/>
+    <col min="14" max="14" width="17.6607142857143" customWidth="1"/>
+    <col min="15" max="15" width="19.3303571428571" customWidth="1"/>
+    <col min="16" max="16" width="11.5803571428571" customWidth="1"/>
+    <col min="17" max="17" width="50.9107142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="56" x14ac:dyDescent="0.25">
+    <row r="1" ht="47" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -849,49 +1387,49 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>46</v>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" ht="88" spans="1:17">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K2">
         <v>64</v>
@@ -900,51 +1438,51 @@
         <v>128</v>
       </c>
       <c r="M2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" ht="106" spans="1:17">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K3">
         <v>16</v>
@@ -953,51 +1491,51 @@
         <v>64</v>
       </c>
       <c r="M3" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="8" t="s">
-        <v>47</v>
+        <v>27</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="P3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" ht="71" spans="1:17">
+      <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="J4" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J4" t="s">
-        <v>34</v>
       </c>
       <c r="K4">
         <v>16</v>
@@ -1006,24 +1544,24 @@
         <v>64</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
-      </c>
-      <c r="N4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>47</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Resource Manager] Adjust X86 to X86_64 in template file
</commit_message>
<xml_diff>
--- a/etc/hostInfo_template.xlsx
+++ b/etc/hostInfo_template.xlsx
@@ -38,13 +38,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t>Arch</t>
     </r>
     <r>
@@ -64,7 +57,8 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>[ARM64/X86]</t>
+      <t>[ARM64/
+X86_64]</t>
     </r>
   </si>
   <si>
@@ -107,6 +101,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>Component Purpose</t>
     </r>
     <r>
@@ -207,7 +208,7 @@
     <t>Rack1</t>
   </si>
   <si>
-    <t>X86</t>
+    <t>X86_64</t>
   </si>
   <si>
     <t>CentOS</t>
@@ -284,12 +285,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -319,23 +320,113 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -343,6 +434,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
@@ -358,151 +458,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -534,187 +494,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -737,15 +697,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -757,21 +708,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,7 +731,31 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -830,152 +790,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -987,20 +947,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1325,7 +1279,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelRow="3"/>
@@ -1390,13 +1344,13 @@
       <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1440,7 +1394,7 @@
       <c r="M2" t="s">
         <v>27</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="N2" s="3" t="s">
         <v>28</v>
       </c>
       <c r="O2" s="3" t="s">
@@ -1449,7 +1403,7 @@
       <c r="P2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1493,7 +1447,7 @@
       <c r="M3" t="s">
         <v>27</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="O3" s="3" t="s">
@@ -1502,7 +1456,7 @@
       <c r="P3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1546,7 +1500,7 @@
       <c r="M4" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="3" t="s">
         <v>28</v>
       </c>
       <c r="O4" s="3" t="s">
@@ -1555,7 +1509,7 @@
       <c r="P4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="6" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Resource Manager] Adjust hostInfo_template.xlsx
</commit_message>
<xml_diff>
--- a/etc/hostInfo_template.xlsx
+++ b/etc/hostInfo_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
   <si>
     <t>Host Name</t>
   </si>
@@ -38,6 +38,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>Arch</t>
     </r>
     <r>
@@ -95,8 +102,9 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>[Database/
-DataMigration]</t>
+      <t>[TiDB/
+DataMigration/
+EnterpriseManager]</t>
     </r>
   </si>
   <si>
@@ -128,7 +136,7 @@
         <charset val="134"/>
       </rPr>
       <t>[Compute/Storage/
-Dispatch]</t>
+Schedule]</t>
     </r>
   </si>
   <si>
@@ -159,19 +167,12 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>[nvme_ssd/
-ssd/sata]</t>
+      <t>[NVMeSSD/
+SSD/SATA]</t>
     </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">Disks
 </t>
     </r>
@@ -183,7 +184,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>[status(optional): 0 - available, 1 - reserved]</t>
+      <t>[status(optional): Available/Reserved]</t>
     </r>
   </si>
   <si>
@@ -220,16 +221,16 @@
     <t>10GE</t>
   </si>
   <si>
-    <t>Database</t>
+    <t>TiDB</t>
   </si>
   <si>
     <t>Compute</t>
   </si>
   <si>
-    <t>ssd</t>
-  </si>
-  <si>
-    <t>[{"name": "vda","capacity": 256,"status": 1, "path": "/", "type": "sata"}, {"name": "vdd", "capacity": 512,"status": 0, "path": "/mnt/vdd", "type":"ssd"}, {"name": "vde","capacity": 1024,"status": 0,"path": "/mnt/vde", "type":"ssd"}]</t>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>[{"name": "vda","capacity": 256,"status": "Reserved", "path": "/", "type": "SATA"}, {"name": "vdd", "capacity": 512,"status": "Available", "path": "/mnt/vdd", "type":"SSD"}, {"name": "vde","capacity": 1024,"status": "Available","path": "/mnt/vde", "type":"SSD"}]</t>
   </si>
   <si>
     <t>HostName2</t>
@@ -250,13 +251,16 @@
     <t>5.2.0</t>
   </si>
   <si>
+    <t>DataMigration</t>
+  </si>
+  <si>
     <t>Storage</t>
   </si>
   <si>
-    <t>nvme_ssd</t>
-  </si>
-  <si>
-    <t>[{"name": "nvme0p1","capacity": 256,"status": 1, "path": "/","type":"nvme_ssd"}, {"name": "nvme0p2", "capacity": 1024,"status": 0, "path": "/mnt/path1", "type": "nvme_ssd"}, {"name": "nvme0p3","capacity": 4096,"status": 0,"path": "/mnt/path2", "type": "nvme_ssd"}]</t>
+    <t>NVMeSSD</t>
+  </si>
+  <si>
+    <t>[{"name": "nvme0p1","capacity": 256,"status": "Reserved", "path": "/","type":"NVMeSSD"}, {"name": "nvme0p2", "capacity": 1024,"status": "Available", "path": "/mnt/path1", "type": "NVMeSSD"}, {"name": "nvme0p3","capacity": 4096,"status": "Available","path": "/mnt/path2", "type": "NVMeSSD"}]</t>
   </si>
   <si>
     <t>HostName3</t>
@@ -271,13 +275,16 @@
     <t>Rack3</t>
   </si>
   <si>
-    <t>Dispatch</t>
-  </si>
-  <si>
-    <t>sata</t>
-  </si>
-  <si>
-    <t>[{"name": "sda","capacity": 256,"status": 1, "path": "/"}, {"name": "sdb", "capacity": 1024,"status": 0, "path": "/mnt/path1"}, {"name": "sdc","capacity": 4096,"status": 0,"path": "/mnt/path2"}]</t>
+    <t>EnterpriseManager</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>SATA</t>
+  </si>
+  <si>
+    <t>[{"name": "sda","capacity": 256,"status": "Reserved", "path": "/"}, {"name": "sdb", "capacity": 1024,"status": "Available", "path": "/mnt/path1"}, {"name": "sdc","capacity": 4096,"status": "Available","path": "/mnt/path2"}]</t>
   </si>
 </sst>
 </file>
@@ -285,10 +292,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -329,6 +336,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -343,9 +358,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,6 +369,14 @@
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -366,13 +388,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -390,61 +428,30 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,9 +465,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,19 +501,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -518,19 +591,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -542,67 +639,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -614,61 +675,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -697,17 +704,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,15 +737,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -756,17 +748,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -785,132 +766,158 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -919,23 +926,23 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -949,9 +956,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1279,7 +1283,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelRow="3"/>
@@ -1301,7 +1305,7 @@
     <col min="17" max="17" width="50.9107142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="47" spans="1:17">
+    <row r="1" ht="61" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1341,20 +1345,20 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="Q1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="88" spans="1:17">
+    <row r="2" ht="106" spans="1:17">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1403,7 +1407,7 @@
       <c r="P2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1448,24 +1452,24 @@
         <v>27</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="6" t="s">
         <v>40</v>
       </c>
+      <c r="Q3" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" ht="71" spans="1:17">
+    <row r="4" ht="88" spans="1:17">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
@@ -1477,10 +1481,10 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>24</v>
@@ -1501,16 +1505,16 @@
         <v>27</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>